<commit_message>
Add .gitignore to ignore 'Koparanov
</commit_message>
<xml_diff>
--- a/Koparanov/info.xlsx
+++ b/Koparanov/info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krisi\Desktop\UKTC\Koparanov\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5303B09-82C2-4F94-A1B1-B030B3E1A3CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F7551C-2DC5-43F8-B0E4-B8E53AA44F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="876" yWindow="2160" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>Пореден номер</t>
   </si>
@@ -54,9 +54,6 @@
     <t>изпълнение</t>
   </si>
   <si>
-    <t>№1</t>
-  </si>
-  <si>
     <t>№2</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>.\chapter_1\System.png</t>
   </si>
   <si>
-    <t>№5</t>
-  </si>
-  <si>
     <t>№6</t>
   </si>
   <si>
@@ -120,9 +114,6 @@
     <t>№14</t>
   </si>
   <si>
-    <t>№15</t>
-  </si>
-  <si>
     <t>стр.103 - 1 зад</t>
   </si>
   <si>
@@ -157,6 +148,159 @@
   </si>
   <si>
     <t>.\chapter_2\escapeCharacter.png</t>
+  </si>
+  <si>
+    <t>стр.104 - 7 зад</t>
+  </si>
+  <si>
+    <t>.\chapter_2\src\chapter_2\triangle.java</t>
+  </si>
+  <si>
+    <t>.\chapter_2\src\chapter_2\heart.java</t>
+  </si>
+  <si>
+    <t>стр.105 - 8 зад</t>
+  </si>
+  <si>
+    <t>.\chapter_2\src\chapter_2\EmployeeRecord.java</t>
+  </si>
+  <si>
+    <t>стр.105 - 9 зад</t>
+  </si>
+  <si>
+    <t>.\chapter_2\src\chapter_2\numSwap.java</t>
+  </si>
+  <si>
+    <t>стр.105 - 10 зад</t>
+  </si>
+  <si>
+    <t>№5 - ch2</t>
+  </si>
+  <si>
+    <t>№1 - ch1</t>
+  </si>
+  <si>
+    <t>№15 - ch3</t>
+  </si>
+  <si>
+    <t>№16</t>
+  </si>
+  <si>
+    <t>№17</t>
+  </si>
+  <si>
+    <t>№18</t>
+  </si>
+  <si>
+    <t>№19</t>
+  </si>
+  <si>
+    <t>№20</t>
+  </si>
+  <si>
+    <t>№21</t>
+  </si>
+  <si>
+    <t>№22</t>
+  </si>
+  <si>
+    <t>№23</t>
+  </si>
+  <si>
+    <t>№24</t>
+  </si>
+  <si>
+    <t>№25</t>
+  </si>
+  <si>
+    <t>№26</t>
+  </si>
+  <si>
+    <t>№27</t>
+  </si>
+  <si>
+    <t>№28</t>
+  </si>
+  <si>
+    <t>№29</t>
+  </si>
+  <si>
+    <t>№30</t>
+  </si>
+  <si>
+    <t>№31</t>
+  </si>
+  <si>
+    <t>№32</t>
+  </si>
+  <si>
+    <t>№33</t>
+  </si>
+  <si>
+    <t>№34</t>
+  </si>
+  <si>
+    <t>№35</t>
+  </si>
+  <si>
+    <t>№36</t>
+  </si>
+  <si>
+    <t>стр.125 - 1 зад</t>
+  </si>
+  <si>
+    <t>стр.125 - 2 зад</t>
+  </si>
+  <si>
+    <t>стр.125 - 3 зад</t>
+  </si>
+  <si>
+    <t>стр.125 - 4 зад</t>
+  </si>
+  <si>
+    <t>стр.125 - 5 зад</t>
+  </si>
+  <si>
+    <t>стр.125 - 6 зад</t>
+  </si>
+  <si>
+    <t>стр.125 - 7 зад</t>
+  </si>
+  <si>
+    <t>стр.125 - 8 зад</t>
+  </si>
+  <si>
+    <t>стр.125 - 9 зад</t>
+  </si>
+  <si>
+    <t>стр.125 - 10 зад</t>
+  </si>
+  <si>
+    <t>стр.125 - 11 зад</t>
+  </si>
+  <si>
+    <t>стр.125 - 12 зад</t>
+  </si>
+  <si>
+    <t>стр.125 - 13 зад</t>
+  </si>
+  <si>
+    <t>.\chapter_3\src\chapter_3\main1.java</t>
+  </si>
+  <si>
+    <t>.\chapter_3\src\chapter_3\main2.java</t>
+  </si>
+  <si>
+    <t>.\chapter_3\src\chapter_3\main3.java</t>
+  </si>
+  <si>
+    <t>.\chapter_3\src\chapter_3\main4.java</t>
+  </si>
+  <si>
+    <t>.\chapter_3\src\chapter_3\main5.java</t>
+  </si>
+  <si>
+    <t>.\chapter_3\src\chapter_3\main6.java</t>
   </si>
 </sst>
 </file>
@@ -498,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,10 +680,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1">
         <v>0.53888888888888886</v>
@@ -552,15 +696,15 @@
         <v>1.388888888888884E-3</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1">
         <v>0.54097222222222219</v>
@@ -569,19 +713,19 @@
         <v>0.54513888888888895</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E16" si="0">D3-C3</f>
+        <f t="shared" ref="E3:E28" si="0">D3-C3</f>
         <v>4.1666666666667629E-3</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1">
         <v>0.54513888888888895</v>
@@ -594,15 +738,15 @@
         <v>3.4722222222220989E-3</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
       </c>
       <c r="C5" s="1">
         <v>0.54861111111111105</v>
@@ -615,15 +759,15 @@
         <v>1.388888888888884E-3</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1">
         <v>0.53472222222222221</v>
@@ -636,15 +780,15 @@
         <v>6.2499999999999778E-3</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1">
         <v>0.54236111111111118</v>
@@ -657,15 +801,15 @@
         <v>6.9444444444433095E-4</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1">
         <v>0.54375000000000007</v>
@@ -678,15 +822,15 @@
         <v>1.388888888888884E-3</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1">
         <v>0.54513888888888895</v>
@@ -699,15 +843,15 @@
         <v>6.9444444444433095E-4</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1">
         <v>0.54583333333333328</v>
@@ -720,15 +864,15 @@
         <v>3.4722222222223209E-3</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1">
         <v>0.55138888888888882</v>
@@ -741,52 +885,346 @@
         <v>2.7777777777778789E-3</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.5541666666666667</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.55694444444444446</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.7777777777777679E-3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.55694444444444446</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.56111111111111112</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666519E-3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.56111111111111112</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.56458333333333333</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.4722222222222099E-3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.57638888888888895</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.4722222222223209E-3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.54791666666666672</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
+        <v>6.2500000000000888E-3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.54791666666666672</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666519E-3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.55972222222222223</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="0"/>
+        <v>7.6388888888888618E-3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.55972222222222223</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.56388888888888888</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666519E-3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.56388888888888888</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="0"/>
+        <v>9.0277777777777457E-3</v>
+      </c>
+      <c r="F20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.57500000000000007</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.57916666666666672</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666519E-3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" s="1">
+        <f>D28-C28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>